<commit_message>
some selenium fixes and fixing mongo aggregate function
</commit_message>
<xml_diff>
--- a/short_squeeze_release_dates.xlsx
+++ b/short_squeeze_release_dates.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="997" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2018" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="2017" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="2016" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="2015" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="2014" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="2019" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="2018" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="2017" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2016" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="2015" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="2014" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="96">
   <si>
     <t xml:space="preserve">NYSE®</t>
   </si>
@@ -44,144 +45,177 @@
     <t xml:space="preserve">January A</t>
   </si>
   <si>
+    <t xml:space="preserve">12/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/13</t>
+  </si>
+  <si>
     <t xml:space="preserve">12/29</t>
   </si>
   <si>
-    <t xml:space="preserve">January B</t>
-  </si>
-  <si>
     <t xml:space="preserve">1/12</t>
   </si>
   <si>
-    <t xml:space="preserve">February A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2/28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April B</t>
-  </si>
-  <si>
     <t xml:space="preserve">4/13</t>
   </si>
   <si>
-    <t xml:space="preserve">May A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June B</t>
-  </si>
-  <si>
     <t xml:space="preserve">6/15</t>
   </si>
   <si>
-    <t xml:space="preserve">July A</t>
-  </si>
-  <si>
     <t xml:space="preserve">6/29</t>
   </si>
   <si>
-    <t xml:space="preserve">July B</t>
-  </si>
-  <si>
     <t xml:space="preserve">7/13</t>
   </si>
   <si>
-    <t xml:space="preserve">August A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September A</t>
-  </si>
-  <si>
     <t xml:space="preserve">8/31</t>
   </si>
   <si>
-    <t xml:space="preserve">September B</t>
-  </si>
-  <si>
     <t xml:space="preserve">9/14</t>
   </si>
   <si>
-    <t xml:space="preserve">October A</t>
-  </si>
-  <si>
     <t xml:space="preserve">9/28</t>
   </si>
   <si>
-    <t xml:space="preserve">October B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December A</t>
-  </si>
-  <si>
     <t xml:space="preserve">11/30</t>
   </si>
   <si>
-    <t xml:space="preserve">December B</t>
-  </si>
-  <si>
     <t xml:space="preserve">12/14</t>
   </si>
   <si>
@@ -215,12 +249,6 @@
     <t xml:space="preserve">12/15</t>
   </si>
   <si>
-    <t xml:space="preserve">12/31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/15</t>
-  </si>
-  <si>
     <t xml:space="preserve">1/29</t>
   </si>
   <si>
@@ -230,22 +258,13 @@
     <t xml:space="preserve">2/29</t>
   </si>
   <si>
-    <t xml:space="preserve">4/15</t>
-  </si>
-  <si>
     <t xml:space="preserve">4/29</t>
   </si>
   <si>
     <t xml:space="preserve">5/13</t>
   </si>
   <si>
-    <t xml:space="preserve">7/15</t>
-  </si>
-  <si>
     <t xml:space="preserve">7/29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9/30</t>
   </si>
   <si>
     <t xml:space="preserve">10/14</t>
@@ -451,18 +470,18 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26:F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -505,16 +524,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>8</v>
@@ -525,16 +544,16 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
@@ -565,16 +584,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>14</v>
@@ -605,16 +624,16 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
@@ -625,16 +644,16 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>20</v>
@@ -705,16 +724,16 @@
         <v>27</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>28</v>
@@ -725,16 +744,16 @@
         <v>29</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>30</v>
@@ -785,16 +804,16 @@
         <v>35</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>36</v>
@@ -805,16 +824,16 @@
         <v>37</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>38</v>
@@ -825,16 +844,16 @@
         <v>39</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>40</v>
@@ -885,16 +904,16 @@
         <v>45</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>46</v>
@@ -905,16 +924,16 @@
         <v>47</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>48</v>
@@ -925,16 +944,16 @@
         <v>49</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>50</v>
@@ -945,16 +964,16 @@
         <v>51</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>52</v>
@@ -971,7 +990,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -986,524 +1005,527 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="A26:F26 A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="1" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="C2" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="D2" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="B6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="D7" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="E7" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="B7" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="B8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="C9" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D9" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="E9" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7" t="s">
+      <c r="B10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="E11" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="E12" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="C13" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="D13" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="E13" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C18" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D18" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E18" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="C15" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D15" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="E15" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C16" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D16" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="E16" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="C17" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="D17" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="E17" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="C18" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="D18" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="E18" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>38</v>
+      <c r="F18" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>59</v>
+      <c r="B19" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D20" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E20" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>60</v>
+      <c r="B20" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="C21" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="D21" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="E21" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>61</v>
+      <c r="B21" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="D22" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="E22" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="F22" s="7" t="s">
+      <c r="B22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="C23" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="D23" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="E23" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="F23" s="7" t="s">
+      <c r="B23" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="C24" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="D24" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="E24" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>50</v>
+      <c r="B24" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="C25" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="D25" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="E25" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>62</v>
+      <c r="B25" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1516,17 +1538,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26:F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1549,19 +1574,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,19 +1594,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +1626,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,19 +1634,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,8 +1665,8 @@
       <c r="E6" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>67</v>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,7 +1706,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,19 +1714,19 @@
         <v>19</v>
       </c>
       <c r="B9" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,19 +1734,19 @@
         <v>21</v>
       </c>
       <c r="B10" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1741,7 +1766,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,19 +1794,19 @@
         <v>27</v>
       </c>
       <c r="B13" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,7 +1826,7 @@
         <v>12</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,19 +1834,19 @@
         <v>31</v>
       </c>
       <c r="B15" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1841,7 +1866,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,7 +1906,7 @@
         <v>12</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,7 +1926,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,19 +1934,19 @@
         <v>41</v>
       </c>
       <c r="B20" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,19 +1954,19 @@
         <v>43</v>
       </c>
       <c r="B21" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,16 +1994,16 @@
         <v>47</v>
       </c>
       <c r="B23" s="6" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" s="6" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D23" s="6" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>48</v>
@@ -1989,19 +2014,19 @@
         <v>49</v>
       </c>
       <c r="B24" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D24" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2021,13 +2046,21 @@
         <v>27</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>62</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2042,15 +2075,18 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A26:F26 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2085,7 +2121,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,7 +2141,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,19 +2149,19 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,19 +2169,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,19 +2189,19 @@
         <v>13</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>77</v>
+        <v>9</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,7 +2221,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,19 +2229,19 @@
         <v>17</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,19 +2249,19 @@
         <v>19</v>
       </c>
       <c r="B9" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,19 +2269,19 @@
         <v>21</v>
       </c>
       <c r="B10" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,19 +2289,19 @@
         <v>23</v>
       </c>
       <c r="B11" s="6" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,7 +2321,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2341,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,19 +2349,19 @@
         <v>29</v>
       </c>
       <c r="B14" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,19 +2369,19 @@
         <v>31</v>
       </c>
       <c r="B15" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,19 +2389,19 @@
         <v>33</v>
       </c>
       <c r="B16" s="6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D16" s="6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2373,19 +2409,19 @@
         <v>35</v>
       </c>
       <c r="B17" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,19 +2429,19 @@
         <v>37</v>
       </c>
       <c r="B18" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D18" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2413,19 +2449,19 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,19 +2469,19 @@
         <v>41</v>
       </c>
       <c r="B20" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2453,19 +2489,19 @@
         <v>43</v>
       </c>
       <c r="B21" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,19 +2509,19 @@
         <v>45</v>
       </c>
       <c r="B22" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,19 +2529,19 @@
         <v>47</v>
       </c>
       <c r="B23" s="6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" s="6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" s="6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,7 +2561,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2533,25 +2569,25 @@
         <v>51</v>
       </c>
       <c r="B25" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C25" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D25" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2566,11 +2602,541 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A26:F26 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="C21" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="C23" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="D25" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E25" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="1" sqref="A26:F26 E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="n">
@@ -2609,7 +3175,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2629,7 +3195,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2669,7 +3235,7 @@
         <v>26</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,7 +3275,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2729,7 +3295,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,7 +3315,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2809,7 +3375,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,7 +3395,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,7 +3415,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +3435,7 @@
         <v>24</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,7 +3495,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2949,7 +3515,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2969,7 +3535,7 @@
         <v>9</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3029,7 +3595,7 @@
         <v>25</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,7 +3615,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3069,13 +3635,13 @@
         <v>24</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>